<commit_message>
feat: implement multi-level pagination, empty course handling, and grid sorting
</commit_message>
<xml_diff>
--- a/public/templates/plantilla_certificados.xlsx
+++ b/public/templates/plantilla_certificados.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L3"/>
+  <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -407,36 +407,24 @@
         <v>Nombre Completo</v>
       </c>
       <c r="B1" t="str">
-        <v>Nombre del Curso</v>
+        <v>ID del Curso</v>
       </c>
       <c r="C1" t="str">
-        <v>Año</v>
+        <v>Identificación</v>
       </c>
       <c r="D1" t="str">
-        <v>Tipo de Curso</v>
+        <v>Email</v>
       </c>
       <c r="E1" t="str">
-        <v>Mes</v>
+        <v>Teléfono</v>
       </c>
       <c r="F1" t="str">
-        <v>Edición</v>
+        <v>Ubicación Física</v>
       </c>
       <c r="G1" t="str">
-        <v>Identificación</v>
+        <v>Estado</v>
       </c>
       <c r="H1" t="str">
-        <v>Email</v>
-      </c>
-      <c r="I1" t="str">
-        <v>Teléfono</v>
-      </c>
-      <c r="J1" t="str">
-        <v>Ubicación Física</v>
-      </c>
-      <c r="K1" t="str">
-        <v>Estado</v>
-      </c>
-      <c r="L1" t="str">
         <v>Origen</v>
       </c>
     </row>
@@ -445,36 +433,24 @@
         <v>Juan Pérez</v>
       </c>
       <c r="B2" t="str">
-        <v>Nutrición y Deporte</v>
-      </c>
-      <c r="C2">
-        <v>2025</v>
+        <v>NUT-1-2025</v>
+      </c>
+      <c r="C2" t="str">
+        <v>0801-1990-12345</v>
       </c>
       <c r="D2" t="str">
-        <v>Curso</v>
-      </c>
-      <c r="E2">
-        <v>3</v>
-      </c>
-      <c r="F2">
-        <v>1</v>
+        <v>juan@ejemplo.com</v>
+      </c>
+      <c r="E2" t="str">
+        <v>50499887766</v>
+      </c>
+      <c r="F2" t="str">
+        <v>Tomo 1 Caja 5</v>
       </c>
       <c r="G2" t="str">
-        <v>0801-1990-12345</v>
+        <v>en_archivo</v>
       </c>
       <c r="H2" t="str">
-        <v>juan@ejemplo.com</v>
-      </c>
-      <c r="I2" t="str">
-        <v>50499887766</v>
-      </c>
-      <c r="J2" t="str">
-        <v>Tomo 1 Caja 5</v>
-      </c>
-      <c r="K2" t="str">
-        <v>en_archivo</v>
-      </c>
-      <c r="L2" t="str">
         <v>nuevo</v>
       </c>
     </row>
@@ -483,42 +459,30 @@
         <v>María García</v>
       </c>
       <c r="B3" t="str">
-        <v>Diplomado en Salud</v>
-      </c>
-      <c r="C3">
-        <v>2024</v>
+        <v>SALUD-2024</v>
+      </c>
+      <c r="C3" t="str">
+        <v/>
       </c>
       <c r="D3" t="str">
-        <v>Diplomado</v>
-      </c>
-      <c r="E3">
-        <v>6</v>
-      </c>
-      <c r="F3">
-        <v>2</v>
+        <v>maria@ejemplo.com</v>
+      </c>
+      <c r="E3" t="str">
+        <v>50488776655</v>
+      </c>
+      <c r="F3" t="str">
+        <v/>
       </c>
       <c r="G3" t="str">
-        <v/>
+        <v>entregado</v>
       </c>
       <c r="H3" t="str">
-        <v>maria@ejemplo.com</v>
-      </c>
-      <c r="I3" t="str">
-        <v>50488776655</v>
-      </c>
-      <c r="J3" t="str">
-        <v/>
-      </c>
-      <c r="K3" t="str">
-        <v>entregado</v>
-      </c>
-      <c r="L3" t="str">
         <v>historico</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:L3"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:H3"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>